<commit_message>
Udpating Self Learning Test Cases
</commit_message>
<xml_diff>
--- a/Self_Learning_Testcases_and_Results/TC_01_NMAP (2.0).xlsx
+++ b/Self_Learning_Testcases_and_Results/TC_01_NMAP (2.0).xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Class12Capstone\Self_Learning_Testcases_and_Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3EF78BDD-2BA3-4DDD-8544-3616A838627B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4500AC-D74E-4D02-B6D3-2972B96F996B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{13FE736A-55E3-4834-9F1C-C4492E998C66}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3EAA6031-D306-4FED-90EA-377CB01D9B4F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Self Learning TC2" sheetId="1" r:id="rId1"/>
+    <sheet name="Self Learning TC1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -62,6 +62,9 @@
     <t>Pass/Fail</t>
   </si>
   <si>
+    <t>TC2: Use NMAP to scan the websites Ipaddress and locate the tracerouts</t>
+  </si>
+  <si>
     <t>1.Initialize the "Zenmap" application from your desktop</t>
   </si>
   <si>
@@ -81,9 +84,6 @@
   </si>
   <si>
     <t>4. Scroll down the information to find the tracerouts. Take note of the which tracerouts are being shown as hackers can use these traceroutes to map how information moved within a company's computer network and then focus their attacks on certain computers</t>
-  </si>
-  <si>
-    <t>TC1: Use NMAP to scan the websites Ipaddress and locate the tracerouts</t>
   </si>
 </sst>
 </file>
@@ -568,11 +568,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE14F094-4D5E-4FD6-BF56-DC5BE62E21FD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D76EB1B-99AF-4FFC-9D69-7334799D424F}">
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -629,13 +629,13 @@
     </row>
     <row r="11" spans="1:5" ht="75.599999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -643,10 +643,10 @@
     <row r="12" spans="1:5" ht="60.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8"/>
       <c r="B12" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -654,17 +654,17 @@
     <row r="13" spans="1:5" ht="72" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10"/>
       <c r="B13" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" ht="87.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="7"/>

</xml_diff>